<commit_message>
Change colours and categories for sectors
</commit_message>
<xml_diff>
--- a/plots-drafts/toy-data/data_tech_green_brown_sectors.xlsx
+++ b/plots-drafts/toy-data/data_tech_green_brown_sectors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/monikafurdyna/Documents/dev/loose_analysis/Executive summary vis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/monikafurdyna/Documents/dev/executive-summary/plots-drafts/toy-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36AFB2C-DC86-0C4C-8957-CB616462D5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF461896-30C1-F24E-97DE-4CA711F18D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33920" yWindow="860" windowWidth="28800" windowHeight="18000" xr2:uid="{A60FAC01-BD50-274F-BCA2-1AA1E13B358C}"/>
+    <workbookView xWindow="-26840" yWindow="1160" windowWidth="28800" windowHeight="18000" xr2:uid="{A60FAC01-BD50-274F-BCA2-1AA1E13B358C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="28">
   <si>
     <t>year</t>
   </si>
@@ -67,18 +67,12 @@
     <t>fossil_fuels</t>
   </si>
   <si>
-    <t>other_brown</t>
-  </si>
-  <si>
     <t>green</t>
   </si>
   <si>
     <t>tech_mix_perc</t>
   </si>
   <si>
-    <t>neutral</t>
-  </si>
-  <si>
     <t>tech</t>
   </si>
   <si>
@@ -119,6 +113,12 @@
   </si>
   <si>
     <t>aviation</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>hydro_and_nuclear</t>
   </si>
 </sst>
 </file>
@@ -476,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD66559C-116D-3942-9BE8-77D8196556AE}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48:I49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,16 +508,16 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -534,16 +534,16 @@
         <v>2022</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G2">
         <v>0.4</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I2">
         <v>1000000</v>
@@ -563,16 +563,16 @@
         <v>2022</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3">
         <v>0.6</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I3">
         <v>1000000</v>
@@ -592,16 +592,16 @@
         <v>2027</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G4">
         <v>0.3</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I4">
         <v>1000000</v>
@@ -621,16 +621,16 @@
         <v>2027</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5">
         <v>0.7</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I5">
         <v>1000000</v>
@@ -644,22 +644,22 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <v>2022</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6">
         <v>0.6</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I6">
         <v>2000000</v>
@@ -673,22 +673,22 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7">
         <v>2022</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7">
         <v>0.4</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I7">
         <v>2000000</v>
@@ -702,22 +702,22 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>2027</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G8">
         <v>0.5</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I8">
         <v>2000000</v>
@@ -731,22 +731,22 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9">
         <v>2027</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>0.5</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I9">
         <v>2000000</v>
@@ -766,7 +766,7 @@
         <v>2022</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
@@ -775,7 +775,7 @@
         <v>0.1</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I10">
         <v>3000000</v>
@@ -795,16 +795,16 @@
         <v>2022</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="G11">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="H11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I11">
         <v>3000000</v>
@@ -824,7 +824,7 @@
         <v>2022</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F12" t="s">
         <v>20</v>
@@ -833,7 +833,7 @@
         <v>0.2</v>
       </c>
       <c r="H12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I12">
         <v>3000000</v>
@@ -853,16 +853,16 @@
         <v>2022</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G13">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="H13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I13">
         <v>3000000</v>
@@ -879,19 +879,19 @@
         <v>6</v>
       </c>
       <c r="D14">
-        <v>2027</v>
+        <v>2022</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="H14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I14">
         <v>3000000</v>
@@ -911,16 +911,16 @@
         <v>2027</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G15">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I15">
         <v>3000000</v>
@@ -940,16 +940,16 @@
         <v>2027</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G16">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="H16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I16">
         <v>3000000</v>
@@ -972,13 +972,13 @@
         <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G17">
-        <v>0.4</v>
+        <v>0.05</v>
       </c>
       <c r="H17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I17">
         <v>3000000</v>
@@ -992,25 +992,25 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D18">
-        <v>2022</v>
+        <v>2027</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="G18">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="H18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I18">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1021,25 +1021,25 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D19">
-        <v>2022</v>
+        <v>2027</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G19">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="H19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I19">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1050,22 +1050,22 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D20">
         <v>2022</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G20">
         <v>0.3</v>
       </c>
       <c r="H20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I20">
         <v>5000000</v>
@@ -1079,7 +1079,7 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D21">
         <v>2022</v>
@@ -1091,10 +1091,10 @@
         <v>21</v>
       </c>
       <c r="G21">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I21">
         <v>5000000</v>
@@ -1108,22 +1108,22 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D22">
-        <v>2027</v>
+        <v>2022</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="G22">
         <v>0.1</v>
       </c>
       <c r="H22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I22">
         <v>5000000</v>
@@ -1137,22 +1137,22 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D23">
-        <v>2027</v>
+        <v>2022</v>
       </c>
       <c r="E23" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G23">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="H23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I23">
         <v>5000000</v>
@@ -1166,22 +1166,22 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D24">
-        <v>2027</v>
+        <v>2022</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G24">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="H24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I24">
         <v>5000000</v>
@@ -1195,7 +1195,7 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D25">
         <v>2027</v>
@@ -1204,13 +1204,13 @@
         <v>13</v>
       </c>
       <c r="F25" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="G25">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="H25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I25">
         <v>5000000</v>
@@ -1224,25 +1224,25 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D26">
-        <v>2022</v>
+        <v>2027</v>
       </c>
       <c r="E26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="G26">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="H26" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I26">
-        <v>50000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -1253,25 +1253,25 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D27">
-        <v>2022</v>
+        <v>2027</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G27">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="H27" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I27">
-        <v>50000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1282,25 +1282,25 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D28">
-        <v>2022</v>
+        <v>2027</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G28">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="H28" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I28">
-        <v>50000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -1311,25 +1311,25 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D29">
         <v>2027</v>
       </c>
       <c r="E29" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F29" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G29">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="H29" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I29">
-        <v>50000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -1343,13 +1343,13 @@
         <v>6</v>
       </c>
       <c r="D30">
-        <v>2027</v>
+        <v>2022</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F30" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="G30">
         <v>0.4</v>
@@ -1372,16 +1372,16 @@
         <v>6</v>
       </c>
       <c r="D31">
-        <v>2027</v>
+        <v>2022</v>
       </c>
       <c r="E31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F31" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G31">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="H31" t="s">
         <v>9</v>
@@ -1398,25 +1398,25 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D32">
         <v>2022</v>
       </c>
       <c r="E32" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F32" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="G32">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H32" t="s">
         <v>9</v>
       </c>
       <c r="I32">
-        <v>20000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -1427,16 +1427,16 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D33">
-        <v>2022</v>
+        <v>2027</v>
       </c>
       <c r="E33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F33" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="G33">
         <v>0.4</v>
@@ -1445,7 +1445,7 @@
         <v>9</v>
       </c>
       <c r="I33">
-        <v>20000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -1456,25 +1456,25 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D34">
-        <v>2022</v>
+        <v>2027</v>
       </c>
       <c r="E34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F34" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G34">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="H34" t="s">
         <v>9</v>
       </c>
       <c r="I34">
-        <v>20000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -1485,16 +1485,16 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D35">
         <v>2027</v>
       </c>
       <c r="E35" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F35" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="G35">
         <v>0.2</v>
@@ -1503,7 +1503,7 @@
         <v>9</v>
       </c>
       <c r="I35">
-        <v>20000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -1514,19 +1514,19 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D36">
-        <v>2027</v>
+        <v>2022</v>
       </c>
       <c r="E36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F36" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="G36">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="H36" t="s">
         <v>9</v>
@@ -1543,19 +1543,19 @@
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D37">
-        <v>2027</v>
+        <v>2022</v>
       </c>
       <c r="E37" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F37" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G37">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="H37" t="s">
         <v>9</v>
@@ -1572,7 +1572,7 @@
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D38">
         <v>2022</v>
@@ -1581,16 +1581,16 @@
         <v>13</v>
       </c>
       <c r="F38" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G38">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="H38" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="I38">
-        <v>100000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -1601,7 +1601,7 @@
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D39">
         <v>2027</v>
@@ -1610,16 +1610,16 @@
         <v>13</v>
       </c>
       <c r="F39" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G39">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="H39" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="I39">
-        <v>100000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -1630,25 +1630,25 @@
         <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D40">
-        <v>2022</v>
+        <v>2027</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
       </c>
       <c r="F40" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G40">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H40" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="I40">
-        <v>500000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -1659,7 +1659,7 @@
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D41">
         <v>2027</v>
@@ -1668,16 +1668,16 @@
         <v>13</v>
       </c>
       <c r="F41" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>0.3</v>
       </c>
       <c r="H41" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="I41">
-        <v>500000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -1694,16 +1694,16 @@
         <v>2022</v>
       </c>
       <c r="E42" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F42" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G42">
         <v>1</v>
       </c>
       <c r="H42" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I42">
         <v>100000</v>
@@ -1723,16 +1723,16 @@
         <v>2027</v>
       </c>
       <c r="E43" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F43" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G43">
         <v>1</v>
       </c>
       <c r="H43" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I43">
         <v>100000</v>
@@ -1746,25 +1746,25 @@
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D44">
         <v>2022</v>
       </c>
       <c r="E44" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F44" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G44">
         <v>1</v>
       </c>
       <c r="H44" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I44">
-        <v>50000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -1775,25 +1775,25 @@
         <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D45">
         <v>2027</v>
       </c>
       <c r="E45" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F45" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G45">
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I45">
-        <v>50000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -1810,16 +1810,16 @@
         <v>2022</v>
       </c>
       <c r="E46" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F46" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G46">
         <v>1</v>
       </c>
       <c r="H46" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I46">
         <v>100000</v>
@@ -1839,16 +1839,16 @@
         <v>2027</v>
       </c>
       <c r="E47" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F47" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G47">
         <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I47">
         <v>100000</v>
@@ -1862,25 +1862,25 @@
         <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D48">
         <v>2022</v>
       </c>
       <c r="E48" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F48" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G48">
         <v>1</v>
       </c>
       <c r="H48" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I48">
-        <v>1000000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -1891,24 +1891,140 @@
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D49">
         <v>2027</v>
       </c>
       <c r="E49" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F49" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="G49">
         <v>1</v>
       </c>
       <c r="H49" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I49">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50">
+        <v>2022</v>
+      </c>
+      <c r="E50" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+      <c r="G50">
+        <v>1</v>
+      </c>
+      <c r="H50" t="s">
+        <v>25</v>
+      </c>
+      <c r="I50">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51">
+        <v>2027</v>
+      </c>
+      <c r="E51" t="s">
+        <v>26</v>
+      </c>
+      <c r="F51" t="s">
+        <v>26</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51" t="s">
+        <v>25</v>
+      </c>
+      <c r="I51">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52">
+        <v>2022</v>
+      </c>
+      <c r="E52" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" t="s">
+        <v>26</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52" t="s">
+        <v>25</v>
+      </c>
+      <c r="I52">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53">
+        <v>2027</v>
+      </c>
+      <c r="E53" t="s">
+        <v>26</v>
+      </c>
+      <c r="F53" t="s">
+        <v>26</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53" t="s">
+        <v>25</v>
+      </c>
+      <c r="I53">
         <v>1000000</v>
       </c>
     </row>

</xml_diff>